<commit_message>
file_validator funcs run continuously
</commit_message>
<xml_diff>
--- a/tests/for_fuker.allprocess_xls/saving_all_modes_test/allprocess_xls_1-1_test_set_dropdown_and_ruleexamplerow.xlsx
+++ b/tests/for_fuker.allprocess_xls/saving_all_modes_test/allprocess_xls_1-1_test_set_dropdown_and_ruleexamplerow.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="340" yWindow="2990" windowWidth="10800" windowHeight="7810" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7810" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -562,19 +562,19 @@
       <c r="D6" s="2" t="inlineStr">
         <is>
           <t>·规则：理工农医类,社会调查报告和人文社科类等3个选项
-·样例：理工农医类</t>
+·样例：社会调查报告和人文社科类</t>
         </is>
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
           <t>·规则：哲学,经济学,法学,教育学,文学等13个选项
-·样例：理学</t>
+·样例：经济学</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
           <t>·规则：哲学,理论经济学,应用经济学,法学等111个选项
-·样例：地质资源与地质工程</t>
+·样例：测绘科学与技术</t>
         </is>
       </c>
       <c r="H6" s="2" t="inlineStr">
@@ -598,19 +598,19 @@
       <c r="L6" s="2" t="inlineStr">
         <is>
           <t>·规则：数学科学学院,物理学院等73个选项
-·样例：北京肿瘤医院</t>
+·样例：汇丰商学院</t>
         </is>
       </c>
       <c r="R6" s="2" t="inlineStr">
         <is>
           <t>·规则：男,女
-·样例：女</t>
+·样例：男</t>
         </is>
       </c>
       <c r="S6" s="2" t="inlineStr">
         <is>
           <t>·规则：数学科学学院,物理学院等73个选项
-·样例：马克思主义学院</t>
+·样例：环境与能源学院</t>
         </is>
       </c>
     </row>

</xml_diff>